<commit_message>
ARIMA and time windows for ARIMA functional
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camiloariasm/Google Drive/laboral/shcp_ing_tribut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A1E93F-BDF5-6743-8AA6-BC551CF60A41}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4965D2-0286-A34C-9763-7075FADEFB05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="920" windowWidth="27640" windowHeight="15820" xr2:uid="{0BB903C8-BC9F-E64B-83B3-CEC963AED77A}"/>
+    <workbookView xWindow="780" yWindow="880" windowWidth="27640" windowHeight="15820" xr2:uid="{0BB903C8-BC9F-E64B-83B3-CEC963AED77A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>Jun 17 - 21</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Ampliar pipeline para que incluya una variable adicional y dos algoritmos de ML. *Para cada modelo es importante comprender como funcionan las covariables en el futuro.*</t>
   </si>
   <si>
-    <t>Cronograma proyecto Predicciomn Ingresos Fiscales</t>
-  </si>
-  <si>
     <t>Notas</t>
   </si>
   <si>
@@ -241,6 +238,15 @@
   </si>
   <si>
     <t>Crear pipeline que descarge,  importe datos de ingresos fiscales, los limpie y convierta para modelar.</t>
+  </si>
+  <si>
+    <t>Cronograma proyecto Predicción Ingresos Fiscales</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OK, incluye ventanas de tiempo y gráficas. Falta pulir código.</t>
   </si>
 </sst>
 </file>
@@ -280,12 +286,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF002060"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -293,6 +293,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -447,19 +453,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -485,28 +485,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -522,6 +510,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,7 +855,7 @@
   <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -851,17 +866,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="22" x14ac:dyDescent="0.25">
-      <c r="B1" s="19">
+      <c r="B1" s="16">
         <v>43634</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>59</v>
+      <c r="C1" s="20" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="3" t="s">
         <v>47</v>
       </c>
@@ -891,13 +906,13 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -924,833 +939,841 @@
       <c r="K4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12">
+      <c r="A5" s="10">
         <v>1</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="9"/>
+      <c r="B5" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="27"/>
     </row>
     <row r="6" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13">
+      <c r="A6" s="11">
         <v>2</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="9"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="27"/>
     </row>
     <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="8">
+      <c r="A7" s="12"/>
+      <c r="B7" s="6">
         <v>2.1</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="9"/>
+      <c r="C7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="27"/>
     </row>
     <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="8">
+      <c r="A8" s="12"/>
+      <c r="B8" s="6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="9"/>
+      <c r="D8" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="27"/>
     </row>
     <row r="9" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="8">
+      <c r="A9" s="12"/>
+      <c r="B9" s="6">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="9"/>
+      <c r="D9" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="27"/>
     </row>
     <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="8">
+      <c r="A10" s="12"/>
+      <c r="B10" s="6">
         <v>2.4</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="9"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="27"/>
     </row>
     <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="8">
+      <c r="A11" s="12"/>
+      <c r="B11" s="6">
         <v>2.5</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="9"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="27"/>
     </row>
     <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="8">
+      <c r="A12" s="12"/>
+      <c r="B12" s="6">
         <v>2.6</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="9"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="27"/>
     </row>
     <row r="13" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="8">
+      <c r="A13" s="12"/>
+      <c r="B13" s="6">
         <v>2.7</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="9"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="27"/>
     </row>
     <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="8">
+      <c r="A14" s="12"/>
+      <c r="B14" s="6">
         <v>2.8</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="9"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="27"/>
     </row>
     <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="10">
+      <c r="A15" s="13"/>
+      <c r="B15" s="8">
         <v>2.9</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="9"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="27"/>
     </row>
     <row r="16" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="13">
+      <c r="A16" s="11">
         <v>3</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="9"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="27"/>
     </row>
     <row r="17" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="8">
+      <c r="A17" s="12"/>
+      <c r="B17" s="6">
         <v>3.1</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="9"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="27"/>
     </row>
     <row r="18" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="8">
+      <c r="A18" s="12"/>
+      <c r="B18" s="6">
         <v>3.2</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="9"/>
+      <c r="C18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="26"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="27"/>
     </row>
     <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="8">
+      <c r="A19" s="12"/>
+      <c r="B19" s="6">
         <v>3.3</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="9"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="27"/>
     </row>
     <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
-      <c r="B20" s="8">
+      <c r="A20" s="12"/>
+      <c r="B20" s="6">
         <v>3.4</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="9"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="27"/>
     </row>
     <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="8">
+      <c r="A21" s="12"/>
+      <c r="B21" s="6">
         <v>3.5</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="9"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="27"/>
     </row>
     <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="8">
+      <c r="A22" s="12"/>
+      <c r="B22" s="6">
         <v>3.6</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="9"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="27"/>
     </row>
     <row r="23" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="8">
+      <c r="A23" s="12"/>
+      <c r="B23" s="6">
         <v>3.7</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="9"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="27"/>
     </row>
     <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="8">
+      <c r="A24" s="12"/>
+      <c r="B24" s="6">
         <v>3.8</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="9"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="27"/>
     </row>
     <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="1">
         <v>3.9</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="9"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="27"/>
     </row>
     <row r="26" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13">
+      <c r="A26" s="11">
         <v>4</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="9"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="27"/>
     </row>
     <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="4">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="9"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="27"/>
     </row>
     <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="4">
         <v>4.2</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="9"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="27"/>
     </row>
     <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="4">
         <v>4.3</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="9"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="27"/>
     </row>
     <row r="30" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="4">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="9"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="27"/>
     </row>
     <row r="31" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="4">
         <v>4.5</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="9"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="27"/>
     </row>
     <row r="32" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="15"/>
-      <c r="B32" s="16">
+      <c r="A32" s="13"/>
+      <c r="B32" s="14">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="9"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="27"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="13">
+      <c r="A33" s="11">
         <v>5</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="9"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="27"/>
     </row>
     <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="14"/>
+      <c r="A34" s="12"/>
       <c r="B34" s="4">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="9"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="27"/>
     </row>
     <row r="35" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="4">
         <v>5.2</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="9"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="27"/>
     </row>
     <row r="36" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="4">
         <v>5.3</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="9"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="27"/>
     </row>
     <row r="37" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
-      <c r="B37" s="16">
+      <c r="A37" s="13"/>
+      <c r="B37" s="14">
         <v>5.4</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="9"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="27"/>
     </row>
     <row r="38" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="13">
+      <c r="A38" s="11">
         <v>6</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="9"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="27"/>
     </row>
     <row r="39" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="4">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="9"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="27"/>
     </row>
     <row r="40" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="15"/>
-      <c r="B40" s="16">
+      <c r="A40" s="13"/>
+      <c r="B40" s="14">
         <v>5.2</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="9"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="27"/>
     </row>
     <row r="41" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="13">
+      <c r="A41" s="11">
         <v>7</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="9"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
+      <c r="L41" s="27"/>
     </row>
     <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
+      <c r="A42" s="12"/>
       <c r="B42" s="4">
         <v>6.1</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="9"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="27"/>
     </row>
     <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
+      <c r="A43" s="12"/>
       <c r="B43" s="4">
         <v>6.2</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="9"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="28"/>
+      <c r="L43" s="27"/>
     </row>
     <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="15"/>
-      <c r="B44" s="16">
+      <c r="A44" s="13"/>
+      <c r="B44" s="14">
         <v>6.3</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="9"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="27"/>
     </row>
     <row r="45" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="13">
+      <c r="A45" s="11">
         <v>8</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="23"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="29"/>
     </row>
     <row r="46" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
+      <c r="A46" s="12"/>
       <c r="B46" s="4">
         <v>7.1</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="24"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="30"/>
     </row>
     <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="14"/>
+      <c r="A47" s="12"/>
       <c r="B47" s="4">
         <v>7.2</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="24"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="30"/>
     </row>
     <row r="48" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="15"/>
-      <c r="B48" s="16">
+      <c r="A48" s="13"/>
+      <c r="B48" s="14">
         <v>7.3</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="25"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="31"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="31"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="32"/>
     </row>
     <row r="51" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="34" x14ac:dyDescent="0.2">
       <c r="C52" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="C53" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="2:3" ht="34" x14ac:dyDescent="0.2">
       <c r="C54" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="2:3" ht="34" x14ac:dyDescent="0.2">
       <c r="C55" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="2:3" ht="34" x14ac:dyDescent="0.2">
       <c r="C56" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ARIMA y SARIMA MODELS
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camiloariasm/Google Drive/laboral/shcp_ing_tribut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4965D2-0286-A34C-9763-7075FADEFB05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF6366F-ED8D-534E-8E27-7B2421EFDB59}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="880" windowWidth="27640" windowHeight="15820" xr2:uid="{0BB903C8-BC9F-E64B-83B3-CEC963AED77A}"/>
+    <workbookView xWindow="780" yWindow="860" windowWidth="27640" windowHeight="15820" activeTab="1" xr2:uid="{0BB903C8-BC9F-E64B-83B3-CEC963AED77A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Jun 18" sheetId="1" r:id="rId1"/>
+    <sheet name="Jun 21" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="72">
   <si>
     <t>Jun 17 - 21</t>
   </si>
@@ -246,7 +247,7 @@
     <t>OK</t>
   </si>
   <si>
-    <t>OK, incluye ventanas de tiempo y gráficas. Falta pulir código.</t>
+    <t>Añadir modelo ARIMA y SARIMA a pipeline</t>
   </si>
 </sst>
 </file>
@@ -445,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -499,18 +500,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -535,8 +524,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E232A735-9CB2-4741-AAC0-A2E603773C7C}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -947,39 +945,39 @@
       <c r="A5" s="10">
         <v>1</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25" t="s">
+      <c r="C5" s="32"/>
+      <c r="D5" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="27"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="23"/>
     </row>
     <row r="6" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>2</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="27"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="23"/>
     </row>
     <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
@@ -989,17 +987,17 @@
       <c r="C7" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="27"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="23"/>
     </row>
     <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
@@ -1009,17 +1007,17 @@
       <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="27"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="23"/>
     </row>
     <row r="9" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
@@ -1029,17 +1027,17 @@
       <c r="C9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="27"/>
+      <c r="D9" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="23"/>
     </row>
     <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
@@ -1049,15 +1047,15 @@
       <c r="C10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="27"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="23"/>
     </row>
     <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
@@ -1067,15 +1065,15 @@
       <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="27"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="23"/>
     </row>
     <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
@@ -1085,15 +1083,15 @@
       <c r="C12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="27"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="23"/>
     </row>
     <row r="13" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
@@ -1103,15 +1101,15 @@
       <c r="C13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="23"/>
     </row>
     <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
@@ -1121,15 +1119,15 @@
       <c r="C14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="27"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="23"/>
     </row>
     <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
@@ -1139,33 +1137,33 @@
       <c r="C15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="27"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="23"/>
     </row>
     <row r="16" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>3</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="27"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="23"/>
     </row>
     <row r="17" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
@@ -1175,15 +1173,15 @@
       <c r="C17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="27"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="23"/>
     </row>
     <row r="18" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
@@ -1193,15 +1191,15 @@
       <c r="C18" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="27"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="23"/>
     </row>
     <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
@@ -1211,15 +1209,15 @@
       <c r="C19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="27"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="23"/>
     </row>
     <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
@@ -1229,15 +1227,15 @@
       <c r="C20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="27"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="23"/>
     </row>
     <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
@@ -1247,15 +1245,15 @@
       <c r="C21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="27"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="23"/>
     </row>
     <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
@@ -1265,15 +1263,15 @@
       <c r="C22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="27"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="23"/>
     </row>
     <row r="23" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
@@ -1283,15 +1281,15 @@
       <c r="C23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="27"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="23"/>
     </row>
     <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
@@ -1301,15 +1299,15 @@
       <c r="C24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="27"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="23"/>
     </row>
     <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
@@ -1319,33 +1317,33 @@
       <c r="C25" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="27"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="23"/>
     </row>
     <row r="26" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>4</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="27"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="23"/>
     </row>
     <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
@@ -1355,15 +1353,15 @@
       <c r="C27" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="27"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="23"/>
     </row>
     <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
@@ -1373,15 +1371,15 @@
       <c r="C28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="27"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="23"/>
     </row>
     <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="12"/>
@@ -1391,15 +1389,15 @@
       <c r="C29" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="27"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="23"/>
     </row>
     <row r="30" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="12"/>
@@ -1409,15 +1407,15 @@
       <c r="C30" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="27"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="23"/>
     </row>
     <row r="31" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="12"/>
@@ -1427,15 +1425,15 @@
       <c r="C31" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="27"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="23"/>
     </row>
     <row r="32" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
@@ -1445,33 +1443,33 @@
       <c r="C32" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="27"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="23"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
         <v>5</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="27"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="23"/>
     </row>
     <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="12"/>
@@ -1481,15 +1479,15 @@
       <c r="C34" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="27"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="23"/>
     </row>
     <row r="35" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="12"/>
@@ -1499,15 +1497,15 @@
       <c r="C35" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="27"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="23"/>
     </row>
     <row r="36" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="12"/>
@@ -1517,15 +1515,15 @@
       <c r="C36" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="27"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="23"/>
     </row>
     <row r="37" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="13"/>
@@ -1535,33 +1533,33 @@
       <c r="C37" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="27"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="23"/>
     </row>
     <row r="38" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
         <v>6</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="26"/>
-      <c r="L38" s="27"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="23"/>
     </row>
     <row r="39" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="12"/>
@@ -1571,15 +1569,15 @@
       <c r="C39" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="28"/>
-      <c r="K39" s="26"/>
-      <c r="L39" s="27"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="23"/>
     </row>
     <row r="40" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="13"/>
@@ -1589,33 +1587,33 @@
       <c r="C40" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="26"/>
-      <c r="L40" s="27"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="23"/>
     </row>
     <row r="41" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
         <v>7</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="27"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="23"/>
     </row>
     <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="12"/>
@@ -1625,15 +1623,15 @@
       <c r="C42" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="26"/>
-      <c r="L42" s="27"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="23"/>
     </row>
     <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="12"/>
@@ -1643,15 +1641,15 @@
       <c r="C43" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
-      <c r="K43" s="28"/>
-      <c r="L43" s="27"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="24"/>
+      <c r="L43" s="23"/>
     </row>
     <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="13"/>
@@ -1661,33 +1659,33 @@
       <c r="C44" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="27"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="24"/>
+      <c r="L44" s="23"/>
     </row>
     <row r="45" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
         <v>8</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
-      <c r="K45" s="26"/>
-      <c r="L45" s="29"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+      <c r="L45" s="25"/>
     </row>
     <row r="46" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="12"/>
@@ -1697,15 +1695,15 @@
       <c r="C46" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
-      <c r="K46" s="26"/>
-      <c r="L46" s="30"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="22"/>
+      <c r="L46" s="26"/>
     </row>
     <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="12"/>
@@ -1715,15 +1713,15 @@
       <c r="C47" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
-      <c r="K47" s="26"/>
-      <c r="L47" s="30"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="26"/>
     </row>
     <row r="48" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="13"/>
@@ -1733,15 +1731,15 @@
       <c r="C48" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="31"/>
-      <c r="I48" s="31"/>
-      <c r="J48" s="31"/>
-      <c r="K48" s="31"/>
-      <c r="L48" s="32"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="27"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="28"/>
     </row>
     <row r="51" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
@@ -1789,4 +1787,1069 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6969A7AB-D898-1F40-B04E-94DD04A5A571}">
+  <dimension ref="A1:L56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="91" customWidth="1"/>
+    <col min="4" max="12" width="6.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="22" x14ac:dyDescent="0.25">
+      <c r="B1" s="16">
+        <v>43637</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>1</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="23"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
+        <v>2</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="23"/>
+    </row>
+    <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
+      <c r="B7" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="23"/>
+    </row>
+    <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="6">
+        <f>B7+0.1</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="23"/>
+    </row>
+    <row r="9" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="12"/>
+      <c r="B9" s="6">
+        <f t="shared" ref="B9:B16" si="0">B8+0.1</f>
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="23"/>
+    </row>
+    <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="6">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="23"/>
+    </row>
+    <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+      <c r="B11" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000004</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="24"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="23"/>
+    </row>
+    <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
+      <c r="B12" s="6">
+        <f t="shared" si="0"/>
+        <v>2.6000000000000005</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="23"/>
+    </row>
+    <row r="13" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="6">
+        <f t="shared" si="0"/>
+        <v>2.7000000000000006</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="23"/>
+    </row>
+    <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="6">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000007</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="23"/>
+    </row>
+    <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="6">
+        <f t="shared" si="0"/>
+        <v>2.9000000000000008</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="23"/>
+    </row>
+    <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="13"/>
+      <c r="B16" s="6">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000009</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="23"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="11">
+        <v>3</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="23"/>
+    </row>
+    <row r="18" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="6">
+        <v>3.1</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="22"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="23"/>
+    </row>
+    <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="6">
+        <f>B18+0.1</f>
+        <v>3.2</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="23"/>
+    </row>
+    <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="6">
+        <f t="shared" ref="B20:B25" si="1">B19+0.1</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="23"/>
+    </row>
+    <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="6">
+        <f t="shared" si="1"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="23"/>
+    </row>
+    <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="6">
+        <f t="shared" si="1"/>
+        <v>3.5000000000000004</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="23"/>
+    </row>
+    <row r="23" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="12"/>
+      <c r="B23" s="6">
+        <f t="shared" si="1"/>
+        <v>3.6000000000000005</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="23"/>
+    </row>
+    <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="12"/>
+      <c r="B24" s="6">
+        <f t="shared" si="1"/>
+        <v>3.7000000000000006</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="23"/>
+    </row>
+    <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="13"/>
+      <c r="B25" s="6">
+        <f t="shared" si="1"/>
+        <v>3.8000000000000007</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="23"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="11">
+        <v>4</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="23"/>
+    </row>
+    <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="12"/>
+      <c r="B27" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="23"/>
+    </row>
+    <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="12"/>
+      <c r="B28" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="23"/>
+    </row>
+    <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="12"/>
+      <c r="B29" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="23"/>
+    </row>
+    <row r="30" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="12"/>
+      <c r="B30" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="23"/>
+    </row>
+    <row r="31" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="12"/>
+      <c r="B31" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="23"/>
+    </row>
+    <row r="32" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="13"/>
+      <c r="B32" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="23"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="11">
+        <v>5</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="23"/>
+    </row>
+    <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="12"/>
+      <c r="B34" s="4">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="23"/>
+    </row>
+    <row r="35" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="12"/>
+      <c r="B35" s="4">
+        <v>5.2</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="23"/>
+    </row>
+    <row r="36" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="12"/>
+      <c r="B36" s="4">
+        <v>5.3</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="23"/>
+    </row>
+    <row r="37" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="13"/>
+      <c r="B37" s="14">
+        <v>5.4</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="23"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="11">
+        <v>6</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="30"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="23"/>
+    </row>
+    <row r="39" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="12"/>
+      <c r="B39" s="4">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="23"/>
+    </row>
+    <row r="40" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="13"/>
+      <c r="B40" s="14">
+        <v>5.2</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="23"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="11">
+        <v>7</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="30"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="23"/>
+    </row>
+    <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="12"/>
+      <c r="B42" s="4">
+        <v>6.1</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="23"/>
+    </row>
+    <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="12"/>
+      <c r="B43" s="4">
+        <v>6.2</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="24"/>
+      <c r="L43" s="23"/>
+    </row>
+    <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="13"/>
+      <c r="B44" s="14">
+        <v>6.3</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="24"/>
+      <c r="L44" s="23"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="11">
+        <v>8</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="30"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+      <c r="L45" s="25"/>
+    </row>
+    <row r="46" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="12"/>
+      <c r="B46" s="4">
+        <v>7.1</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="22"/>
+      <c r="L46" s="26"/>
+    </row>
+    <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="12"/>
+      <c r="B47" s="4">
+        <v>7.2</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="26"/>
+    </row>
+    <row r="48" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="13"/>
+      <c r="B48" s="14">
+        <v>7.3</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="27"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="28"/>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+    </row>
+    <row r="51" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+    </row>
+    <row r="52" spans="2:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+    </row>
+    <row r="53" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+    </row>
+    <row r="54" spans="2:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+    </row>
+    <row r="55" spans="2:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="B55" s="1"/>
+      <c r="C55" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+    </row>
+    <row r="56" spans="2:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="B56" s="1"/>
+      <c r="C56" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B38:C38"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ELASTICITY y PROPHET CASI LISTOS
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camiloariasm/Google Drive/laboral/shcp_ing_tribut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF6366F-ED8D-534E-8E27-7B2421EFDB59}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFD91C4-2F00-6444-84B0-A4499E3AD7EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="860" windowWidth="27640" windowHeight="15820" activeTab="1" xr2:uid="{0BB903C8-BC9F-E64B-83B3-CEC963AED77A}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="72">
   <si>
     <t>Jun 17 - 21</t>
   </si>
@@ -1793,8 +1793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6969A7AB-D898-1F40-B04E-94DD04A5A571}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2013,7 +2013,9 @@
       <c r="C10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="24"/>
+      <c r="D10" s="24" t="s">
+        <v>70</v>
+      </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>

</xml_diff>